<commit_message>
update model parameters, add code for plotting decision boundary
</commit_message>
<xml_diff>
--- a/proodos.xlsx
+++ b/proodos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14080" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>KNN</t>
   </si>
@@ -40,13 +40,61 @@
   </si>
   <si>
     <t xml:space="preserve"> 0.648183398163</t>
+  </si>
+  <si>
+    <t>SVM</t>
+  </si>
+  <si>
+    <t>normalized</t>
+  </si>
+  <si>
+    <t>max_depth=10, splitter='best', min_samples_split=81</t>
+  </si>
+  <si>
+    <t>NORM?</t>
+  </si>
+  <si>
+    <t>PARAM (non-default)</t>
+  </si>
+  <si>
+    <t>n_neighbors=10, weights= 'distance',metric='manhattan'</t>
+  </si>
+  <si>
+    <t>multi_class='multinomial',  max_iter=500, solver="newton-cg",C=1</t>
+  </si>
+  <si>
+    <t>n_estimators=250, max_depth=None, bootstrap=False, class_weight="balanced", n_jobs=4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5796</t>
+  </si>
+  <si>
+    <t>?????????</t>
+  </si>
+  <si>
+    <t>NEURAL NETWORKS</t>
+  </si>
+  <si>
+    <t>0.545973682033</t>
+  </si>
+  <si>
+    <t>C=1000, kernel='poly', degree=10, coef0=3</t>
+  </si>
+  <si>
+    <t>0.67218406025</t>
+  </si>
+  <si>
+    <t>Ensemble</t>
+  </si>
+  <si>
+    <t>0.675080691881</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -61,13 +109,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -79,14 +139,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -416,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -428,35 +491,92 @@
     <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="2" t="s">
         <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>